<commit_message>
Conditional Statements added to FP 1, minor
</commit_message>
<xml_diff>
--- a/Sesi 12/FINALPROJECTS2010161213281-220627-220853/FINAL PROJECTS/API/ScenarioTestDocs-20220706-F.X. Airell Valerio Satrio W (API).xlsx
+++ b/Sesi 12/FINALPROJECTS2010161213281-220627-220853/FINAL PROJECTS/API/ScenarioTestDocs-20220706-F.X. Airell Valerio Satrio W (API).xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\095068\Documents\Automation Testing with Katalon Studio\Sesi 12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\095068\Documents\Automation Testing with Katalon Studio\Sesi 12\FINALPROJECTS2010161213281-220627-220853\FINAL PROJECTS\API\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -46,6 +46,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
+[Solved] With Addition of Conditional Statement
 1. Data is relatively dynamic to be used for Data Driven Testing using static data storage (Excel)
 2. Two attempts in using this method showed that it's not suitable for DDT with Excel, hence it's declared Failed for further testing method suitable</t>
         </r>
@@ -3354,73 +3355,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3429,29 +3367,35 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3486,11 +3430,68 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3710,7 +3711,7 @@
   <dimension ref="A1:AB674"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3732,22 +3733,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68"/>
+      <c r="B1" s="49"/>
       <c r="C1" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1" s="22"/>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="68"/>
-      <c r="G1" s="69" t="s">
+      <c r="F1" s="49"/>
+      <c r="G1" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="70"/>
+      <c r="H1" s="51"/>
       <c r="I1" s="22"/>
       <c r="J1" s="22"/>
       <c r="K1" s="22"/>
@@ -3800,22 +3801,22 @@
       <c r="AB2" s="22"/>
     </row>
     <row r="3" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="68"/>
+      <c r="B3" s="49"/>
       <c r="C3" s="6" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="22"/>
-      <c r="E3" s="72" t="s">
+      <c r="E3" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="68"/>
-      <c r="G3" s="73">
-        <v>44022</v>
-      </c>
-      <c r="H3" s="70"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="54">
+        <v>44024</v>
+      </c>
+      <c r="H3" s="51"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
@@ -3868,15 +3869,15 @@
       <c r="AB4" s="22"/>
     </row>
     <row r="5" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="68"/>
+      <c r="B5" s="49"/>
       <c r="C5" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D5" s="22"/>
-      <c r="E5" s="74" t="s">
+      <c r="E5" s="55" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="10" t="s">
@@ -3914,14 +3915,14 @@
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
-      <c r="E6" s="75"/>
+      <c r="E6" s="56"/>
       <c r="F6" s="13">
         <f>COUNTIF(I:I,"Passed")</f>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G6" s="14">
         <f>COUNTIF(I:I,"Failed")</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="22"/>
@@ -3985,10 +3986,10 @@
       <c r="C8" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="76" t="s">
+      <c r="D8" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="77"/>
+      <c r="E8" s="58"/>
       <c r="F8" s="18" t="s">
         <v>13</v>
       </c>
@@ -4022,13 +4023,13 @@
       <c r="AB8" s="22"/>
     </row>
     <row r="9" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="60" t="s">
         <v>138</v>
       </c>
       <c r="D9" s="41" t="s">
@@ -4041,13 +4042,13 @@
       <c r="I9" s="23"/>
     </row>
     <row r="10" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="34"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="43" t="s">
+      <c r="A10" s="47"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="E10" s="44"/>
+      <c r="E10" s="35"/>
       <c r="F10" s="21"/>
       <c r="G10" s="21" t="s">
         <v>139</v>
@@ -4058,13 +4059,13 @@
       <c r="I10" s="21"/>
     </row>
     <row r="11" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="34"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="43" t="s">
+      <c r="A11" s="47"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="E11" s="44"/>
+      <c r="E11" s="35"/>
       <c r="F11" s="21"/>
       <c r="G11" s="21" t="s">
         <v>141</v>
@@ -4077,11 +4078,11 @@
       </c>
     </row>
     <row r="12" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="37" t="s">
+      <c r="B12" s="62"/>
+      <c r="C12" s="60" t="s">
         <v>143</v>
       </c>
       <c r="D12" s="41" t="s">
@@ -4094,13 +4095,13 @@
       <c r="I12" s="23"/>
     </row>
     <row r="13" spans="1:28" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="34"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="63" t="s">
+      <c r="A13" s="47"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="38" t="s">
         <v>148</v>
       </c>
-      <c r="E13" s="55"/>
+      <c r="E13" s="39"/>
       <c r="F13" s="21"/>
       <c r="G13" s="21" t="s">
         <v>151</v>
@@ -4113,11 +4114,11 @@
       </c>
     </row>
     <row r="14" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="37" t="s">
+      <c r="B14" s="62"/>
+      <c r="C14" s="60" t="s">
         <v>144</v>
       </c>
       <c r="D14" s="41" t="s">
@@ -4130,13 +4131,13 @@
       <c r="I14" s="23"/>
     </row>
     <row r="15" spans="1:28" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="34"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="63" t="s">
+      <c r="A15" s="47"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="38" t="s">
         <v>148</v>
       </c>
-      <c r="E15" s="55"/>
+      <c r="E15" s="39"/>
       <c r="F15" s="21"/>
       <c r="G15" s="21" t="s">
         <v>151</v>
@@ -4149,11 +4150,11 @@
       </c>
     </row>
     <row r="16" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="37" t="s">
+      <c r="B16" s="62"/>
+      <c r="C16" s="60" t="s">
         <v>145</v>
       </c>
       <c r="D16" s="41" t="s">
@@ -4166,13 +4167,13 @@
       <c r="I16" s="23"/>
     </row>
     <row r="17" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="34"/>
-      <c r="B17" s="39"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="66" t="s">
+      <c r="A17" s="47"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="43" t="s">
         <v>148</v>
       </c>
-      <c r="E17" s="51"/>
+      <c r="E17" s="44"/>
       <c r="F17" s="24"/>
       <c r="G17" s="24" t="s">
         <v>151</v>
@@ -4185,30 +4186,30 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="36" t="s">
+      <c r="B18" s="62"/>
+      <c r="C18" s="59" t="s">
         <v>146</v>
       </c>
-      <c r="D18" s="43" t="s">
+      <c r="D18" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="E18" s="44"/>
+      <c r="E18" s="35"/>
       <c r="F18" s="21"/>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
       <c r="I18" s="21"/>
     </row>
     <row r="19" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="34"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="66" t="s">
+      <c r="A19" s="47"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="E19" s="51"/>
+      <c r="E19" s="44"/>
       <c r="F19" s="24"/>
       <c r="G19" s="24" t="s">
         <v>152</v>
@@ -4221,30 +4222,30 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="39"/>
-      <c r="C20" s="36" t="s">
+      <c r="B20" s="62"/>
+      <c r="C20" s="59" t="s">
         <v>149</v>
       </c>
-      <c r="D20" s="43" t="s">
+      <c r="D20" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="E20" s="44"/>
+      <c r="E20" s="35"/>
       <c r="F20" s="21"/>
       <c r="G20" s="21"/>
       <c r="H20" s="21"/>
       <c r="I20" s="21"/>
     </row>
     <row r="21" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="34"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="66" t="s">
+      <c r="A21" s="47"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="60"/>
+      <c r="D21" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="E21" s="51"/>
+      <c r="E21" s="44"/>
       <c r="F21" s="24"/>
       <c r="G21" s="24" t="s">
         <v>152</v>
@@ -4257,30 +4258,30 @@
       </c>
     </row>
     <row r="22" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="36" t="s">
+      <c r="B22" s="62"/>
+      <c r="C22" s="59" t="s">
         <v>150</v>
       </c>
-      <c r="D22" s="43" t="s">
+      <c r="D22" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="E22" s="44"/>
+      <c r="E22" s="35"/>
       <c r="F22" s="21"/>
       <c r="G22" s="21"/>
       <c r="H22" s="21"/>
       <c r="I22" s="21"/>
     </row>
     <row r="23" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="34"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="66" t="s">
+      <c r="A23" s="47"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="E23" s="51"/>
+      <c r="E23" s="44"/>
       <c r="F23" s="24"/>
       <c r="G23" s="24" t="s">
         <v>152</v>
@@ -4293,13 +4294,13 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="B24" s="39" t="s">
+      <c r="B24" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="65" t="s">
+      <c r="C24" s="63" t="s">
         <v>154</v>
       </c>
       <c r="D24" s="41" t="s">
@@ -4312,13 +4313,13 @@
       <c r="I24" s="23"/>
     </row>
     <row r="25" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="39"/>
-      <c r="B25" s="39"/>
-      <c r="C25" s="65"/>
-      <c r="D25" s="43" t="s">
+      <c r="A25" s="62"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="E25" s="44"/>
+      <c r="E25" s="35"/>
       <c r="F25" s="21"/>
       <c r="G25" s="21" t="s">
         <v>139</v>
@@ -4329,13 +4330,13 @@
       <c r="I25" s="21"/>
     </row>
     <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="39"/>
-      <c r="B26" s="39"/>
+      <c r="A26" s="62"/>
+      <c r="B26" s="62"/>
       <c r="C26" s="64"/>
-      <c r="D26" s="43" t="s">
+      <c r="D26" s="34" t="s">
         <v>212</v>
       </c>
-      <c r="E26" s="44"/>
+      <c r="E26" s="35"/>
       <c r="F26" s="21"/>
       <c r="G26" s="21" t="s">
         <v>213</v>
@@ -4348,11 +4349,11 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="62" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="39"/>
-      <c r="C27" s="37" t="s">
+      <c r="B27" s="62"/>
+      <c r="C27" s="60" t="s">
         <v>199</v>
       </c>
       <c r="D27" s="41" t="s">
@@ -4365,13 +4366,13 @@
       <c r="I27" s="23"/>
     </row>
     <row r="28" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="39"/>
-      <c r="B28" s="39"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="43" t="s">
+      <c r="A28" s="62"/>
+      <c r="B28" s="62"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="E28" s="44"/>
+      <c r="E28" s="35"/>
       <c r="F28" s="21"/>
       <c r="G28" s="21" t="s">
         <v>139</v>
@@ -4382,13 +4383,13 @@
       <c r="I28" s="21"/>
     </row>
     <row r="29" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="39"/>
-      <c r="B29" s="39"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="43" t="s">
+      <c r="A29" s="62"/>
+      <c r="B29" s="62"/>
+      <c r="C29" s="61"/>
+      <c r="D29" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="E29" s="44"/>
+      <c r="E29" s="35"/>
       <c r="F29" s="21"/>
       <c r="G29" s="21" t="s">
         <v>215</v>
@@ -4397,15 +4398,15 @@
         <v>215</v>
       </c>
       <c r="I29" s="21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="37" t="s">
+      <c r="B30" s="62"/>
+      <c r="C30" s="60" t="s">
         <v>200</v>
       </c>
       <c r="D30" s="41" t="s">
@@ -4418,13 +4419,13 @@
       <c r="I30" s="23"/>
     </row>
     <row r="31" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="34"/>
-      <c r="B31" s="39"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="43" t="s">
+      <c r="A31" s="47"/>
+      <c r="B31" s="62"/>
+      <c r="C31" s="60"/>
+      <c r="D31" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="E31" s="44"/>
+      <c r="E31" s="35"/>
       <c r="F31" s="21"/>
       <c r="G31" s="21" t="s">
         <v>139</v>
@@ -4435,13 +4436,13 @@
       <c r="I31" s="21"/>
     </row>
     <row r="32" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="34"/>
-      <c r="B32" s="39"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="43" t="s">
+      <c r="A32" s="47"/>
+      <c r="B32" s="62"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="E32" s="44"/>
+      <c r="E32" s="35"/>
       <c r="F32" s="21"/>
       <c r="G32" s="21" t="s">
         <v>215</v>
@@ -4454,11 +4455,11 @@
       </c>
     </row>
     <row r="33" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="B33" s="39"/>
-      <c r="C33" s="37" t="s">
+      <c r="B33" s="62"/>
+      <c r="C33" s="60" t="s">
         <v>201</v>
       </c>
       <c r="D33" s="41" t="s">
@@ -4471,13 +4472,13 @@
       <c r="I33" s="23"/>
     </row>
     <row r="34" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="34"/>
-      <c r="B34" s="39"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="43" t="s">
+      <c r="A34" s="47"/>
+      <c r="B34" s="62"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="E34" s="44"/>
+      <c r="E34" s="35"/>
       <c r="F34" s="21"/>
       <c r="G34" s="21" t="s">
         <v>139</v>
@@ -4488,13 +4489,13 @@
       <c r="I34" s="21"/>
     </row>
     <row r="35" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="34"/>
-      <c r="B35" s="39"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="57" t="s">
+      <c r="A35" s="47"/>
+      <c r="B35" s="62"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="E35" s="58"/>
+      <c r="E35" s="37"/>
       <c r="F35" s="24"/>
       <c r="G35" s="24" t="s">
         <v>215</v>
@@ -4507,30 +4508,30 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="B36" s="39"/>
-      <c r="C36" s="36" t="s">
+      <c r="B36" s="62"/>
+      <c r="C36" s="59" t="s">
         <v>201</v>
       </c>
-      <c r="D36" s="43" t="s">
+      <c r="D36" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="E36" s="44"/>
+      <c r="E36" s="35"/>
       <c r="F36" s="21"/>
       <c r="G36" s="21"/>
       <c r="H36" s="21"/>
       <c r="I36" s="21"/>
     </row>
     <row r="37" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="34"/>
-      <c r="B37" s="39"/>
-      <c r="C37" s="37"/>
-      <c r="D37" s="43" t="s">
+      <c r="A37" s="47"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="60"/>
+      <c r="D37" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="E37" s="44"/>
+      <c r="E37" s="35"/>
       <c r="F37" s="21"/>
       <c r="G37" s="21" t="s">
         <v>139</v>
@@ -4541,13 +4542,13 @@
       <c r="I37" s="21"/>
     </row>
     <row r="38" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="34"/>
-      <c r="B38" s="39"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="57" t="s">
+      <c r="A38" s="47"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="60"/>
+      <c r="D38" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="E38" s="58"/>
+      <c r="E38" s="37"/>
       <c r="F38" s="24"/>
       <c r="G38" s="24" t="s">
         <v>215</v>
@@ -4560,30 +4561,30 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="34" t="s">
+      <c r="A39" s="47" t="s">
         <v>127</v>
       </c>
-      <c r="B39" s="39"/>
-      <c r="C39" s="36" t="s">
+      <c r="B39" s="62"/>
+      <c r="C39" s="59" t="s">
         <v>201</v>
       </c>
-      <c r="D39" s="43" t="s">
+      <c r="D39" s="34" t="s">
         <v>205</v>
       </c>
-      <c r="E39" s="44"/>
+      <c r="E39" s="35"/>
       <c r="F39" s="21"/>
       <c r="G39" s="21"/>
       <c r="H39" s="21"/>
       <c r="I39" s="21"/>
     </row>
     <row r="40" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="34"/>
-      <c r="B40" s="39"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="43" t="s">
+      <c r="A40" s="47"/>
+      <c r="B40" s="62"/>
+      <c r="C40" s="60"/>
+      <c r="D40" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="E40" s="44"/>
+      <c r="E40" s="35"/>
       <c r="F40" s="21"/>
       <c r="G40" s="21" t="s">
         <v>139</v>
@@ -4594,13 +4595,13 @@
       <c r="I40" s="21"/>
     </row>
     <row r="41" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="34"/>
-      <c r="B41" s="39"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="57" t="s">
+      <c r="A41" s="47"/>
+      <c r="B41" s="62"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="E41" s="58"/>
+      <c r="E41" s="37"/>
       <c r="F41" s="24"/>
       <c r="G41" s="24" t="s">
         <v>215</v>
@@ -4613,30 +4614,30 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="47" t="s">
         <v>128</v>
       </c>
-      <c r="B42" s="39"/>
-      <c r="C42" s="36" t="s">
+      <c r="B42" s="62"/>
+      <c r="C42" s="59" t="s">
         <v>201</v>
       </c>
-      <c r="D42" s="43" t="s">
+      <c r="D42" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="E42" s="44"/>
+      <c r="E42" s="35"/>
       <c r="F42" s="21"/>
       <c r="G42" s="21"/>
       <c r="H42" s="21"/>
       <c r="I42" s="21"/>
     </row>
     <row r="43" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="34"/>
-      <c r="B43" s="39"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="43" t="s">
+      <c r="A43" s="47"/>
+      <c r="B43" s="62"/>
+      <c r="C43" s="60"/>
+      <c r="D43" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="E43" s="44"/>
+      <c r="E43" s="35"/>
       <c r="F43" s="21"/>
       <c r="G43" s="21" t="s">
         <v>139</v>
@@ -4647,13 +4648,13 @@
       <c r="I43" s="21"/>
     </row>
     <row r="44" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="34"/>
-      <c r="B44" s="39"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="57" t="s">
+      <c r="A44" s="47"/>
+      <c r="B44" s="62"/>
+      <c r="C44" s="60"/>
+      <c r="D44" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="E44" s="58"/>
+      <c r="E44" s="37"/>
       <c r="F44" s="24"/>
       <c r="G44" s="24" t="s">
         <v>215</v>
@@ -4666,11 +4667,11 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="34" t="s">
+      <c r="A45" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="B45" s="39"/>
-      <c r="C45" s="37" t="s">
+      <c r="B45" s="62"/>
+      <c r="C45" s="60" t="s">
         <v>201</v>
       </c>
       <c r="D45" s="41" t="s">
@@ -4683,13 +4684,13 @@
       <c r="I45" s="23"/>
     </row>
     <row r="46" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="34"/>
-      <c r="B46" s="39"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="43" t="s">
+      <c r="A46" s="47"/>
+      <c r="B46" s="62"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="E46" s="44"/>
+      <c r="E46" s="35"/>
       <c r="F46" s="21"/>
       <c r="G46" s="21" t="s">
         <v>139</v>
@@ -4700,13 +4701,13 @@
       <c r="I46" s="21"/>
     </row>
     <row r="47" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="34"/>
-      <c r="B47" s="39"/>
-      <c r="C47" s="38"/>
-      <c r="D47" s="43" t="s">
+      <c r="A47" s="47"/>
+      <c r="B47" s="62"/>
+      <c r="C47" s="61"/>
+      <c r="D47" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="E47" s="44"/>
+      <c r="E47" s="35"/>
       <c r="F47" s="21"/>
       <c r="G47" s="21" t="s">
         <v>215</v>
@@ -4719,11 +4720,11 @@
       </c>
     </row>
     <row r="48" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="34" t="s">
+      <c r="A48" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="B48" s="39"/>
-      <c r="C48" s="37" t="s">
+      <c r="B48" s="62"/>
+      <c r="C48" s="60" t="s">
         <v>201</v>
       </c>
       <c r="D48" s="41" t="s">
@@ -4736,13 +4737,13 @@
       <c r="I48" s="23"/>
     </row>
     <row r="49" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="34"/>
-      <c r="B49" s="39"/>
-      <c r="C49" s="37"/>
-      <c r="D49" s="43" t="s">
+      <c r="A49" s="47"/>
+      <c r="B49" s="62"/>
+      <c r="C49" s="60"/>
+      <c r="D49" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="E49" s="44"/>
+      <c r="E49" s="35"/>
       <c r="F49" s="21"/>
       <c r="G49" s="21" t="s">
         <v>139</v>
@@ -4753,13 +4754,13 @@
       <c r="I49" s="21"/>
     </row>
     <row r="50" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="34"/>
-      <c r="B50" s="39"/>
-      <c r="C50" s="38"/>
-      <c r="D50" s="43" t="s">
+      <c r="A50" s="47"/>
+      <c r="B50" s="62"/>
+      <c r="C50" s="61"/>
+      <c r="D50" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="E50" s="44"/>
+      <c r="E50" s="35"/>
       <c r="F50" s="21"/>
       <c r="G50" s="21" t="s">
         <v>215</v>
@@ -4772,11 +4773,11 @@
       </c>
     </row>
     <row r="51" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="34" t="s">
+      <c r="A51" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="B51" s="39"/>
-      <c r="C51" s="37" t="s">
+      <c r="B51" s="62"/>
+      <c r="C51" s="60" t="s">
         <v>201</v>
       </c>
       <c r="D51" s="41" t="s">
@@ -4789,13 +4790,13 @@
       <c r="I51" s="23"/>
     </row>
     <row r="52" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="34"/>
-      <c r="B52" s="39"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="43" t="s">
+      <c r="A52" s="47"/>
+      <c r="B52" s="62"/>
+      <c r="C52" s="60"/>
+      <c r="D52" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="E52" s="44"/>
+      <c r="E52" s="35"/>
       <c r="F52" s="21"/>
       <c r="G52" s="21" t="s">
         <v>139</v>
@@ -4806,13 +4807,13 @@
       <c r="I52" s="21"/>
     </row>
     <row r="53" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="34"/>
-      <c r="B53" s="39"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="57" t="s">
+      <c r="A53" s="47"/>
+      <c r="B53" s="62"/>
+      <c r="C53" s="60"/>
+      <c r="D53" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="E53" s="58"/>
+      <c r="E53" s="37"/>
       <c r="F53" s="24"/>
       <c r="G53" s="24" t="s">
         <v>215</v>
@@ -4825,30 +4826,30 @@
       </c>
     </row>
     <row r="54" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="34" t="s">
+      <c r="A54" s="47" t="s">
         <v>132</v>
       </c>
-      <c r="B54" s="39"/>
-      <c r="C54" s="36" t="s">
+      <c r="B54" s="62"/>
+      <c r="C54" s="59" t="s">
         <v>201</v>
       </c>
-      <c r="D54" s="43" t="s">
+      <c r="D54" s="34" t="s">
         <v>210</v>
       </c>
-      <c r="E54" s="44"/>
+      <c r="E54" s="35"/>
       <c r="F54" s="21"/>
       <c r="G54" s="21"/>
       <c r="H54" s="21"/>
       <c r="I54" s="21"/>
     </row>
     <row r="55" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="34"/>
-      <c r="B55" s="39"/>
-      <c r="C55" s="37"/>
-      <c r="D55" s="43" t="s">
+      <c r="A55" s="47"/>
+      <c r="B55" s="62"/>
+      <c r="C55" s="60"/>
+      <c r="D55" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="E55" s="44"/>
+      <c r="E55" s="35"/>
       <c r="F55" s="21"/>
       <c r="G55" s="21" t="s">
         <v>139</v>
@@ -4859,13 +4860,13 @@
       <c r="I55" s="21"/>
     </row>
     <row r="56" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="34"/>
-      <c r="B56" s="39"/>
-      <c r="C56" s="37"/>
-      <c r="D56" s="57" t="s">
+      <c r="A56" s="47"/>
+      <c r="B56" s="62"/>
+      <c r="C56" s="60"/>
+      <c r="D56" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="E56" s="58"/>
+      <c r="E56" s="37"/>
       <c r="F56" s="24"/>
       <c r="G56" s="24" t="s">
         <v>215</v>
@@ -4878,30 +4879,30 @@
       </c>
     </row>
     <row r="57" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="34" t="s">
+      <c r="A57" s="47" t="s">
         <v>184</v>
       </c>
-      <c r="B57" s="39"/>
-      <c r="C57" s="36" t="s">
+      <c r="B57" s="62"/>
+      <c r="C57" s="59" t="s">
         <v>201</v>
       </c>
-      <c r="D57" s="43" t="s">
+      <c r="D57" s="34" t="s">
         <v>211</v>
       </c>
-      <c r="E57" s="44"/>
+      <c r="E57" s="35"/>
       <c r="F57" s="21"/>
       <c r="G57" s="21"/>
       <c r="H57" s="21"/>
       <c r="I57" s="21"/>
     </row>
     <row r="58" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="34"/>
-      <c r="B58" s="39"/>
-      <c r="C58" s="37"/>
-      <c r="D58" s="43" t="s">
+      <c r="A58" s="47"/>
+      <c r="B58" s="62"/>
+      <c r="C58" s="60"/>
+      <c r="D58" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="E58" s="44"/>
+      <c r="E58" s="35"/>
       <c r="F58" s="21"/>
       <c r="G58" s="21" t="s">
         <v>139</v>
@@ -4912,13 +4913,13 @@
       <c r="I58" s="21"/>
     </row>
     <row r="59" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="34"/>
-      <c r="B59" s="39"/>
-      <c r="C59" s="37"/>
-      <c r="D59" s="57" t="s">
+      <c r="A59" s="47"/>
+      <c r="B59" s="62"/>
+      <c r="C59" s="60"/>
+      <c r="D59" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="E59" s="58"/>
+      <c r="E59" s="37"/>
       <c r="F59" s="24"/>
       <c r="G59" s="24" t="s">
         <v>215</v>
@@ -4931,13 +4932,13 @@
       </c>
     </row>
     <row r="60" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="34" t="s">
+      <c r="A60" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="B60" s="40" t="s">
+      <c r="B60" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="C60" s="65" t="s">
+      <c r="C60" s="63" t="s">
         <v>156</v>
       </c>
       <c r="D60" s="41" t="s">
@@ -4950,13 +4951,13 @@
       <c r="I60" s="23"/>
     </row>
     <row r="61" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="34"/>
-      <c r="B61" s="52"/>
-      <c r="C61" s="65"/>
-      <c r="D61" s="43" t="s">
+      <c r="A61" s="47"/>
+      <c r="B61" s="74"/>
+      <c r="C61" s="63"/>
+      <c r="D61" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="E61" s="44"/>
+      <c r="E61" s="35"/>
       <c r="F61" s="21"/>
       <c r="G61" s="21" t="s">
         <v>139</v>
@@ -4967,13 +4968,13 @@
       <c r="I61" s="21"/>
     </row>
     <row r="62" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="34"/>
-      <c r="B62" s="52"/>
+      <c r="A62" s="47"/>
+      <c r="B62" s="74"/>
       <c r="C62" s="64"/>
-      <c r="D62" s="43" t="s">
+      <c r="D62" s="34" t="s">
         <v>216</v>
       </c>
-      <c r="E62" s="44"/>
+      <c r="E62" s="35"/>
       <c r="F62" s="21"/>
       <c r="G62" s="21" t="s">
         <v>217</v>
@@ -4986,11 +4987,11 @@
       </c>
     </row>
     <row r="63" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="34" t="s">
+      <c r="A63" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="B63" s="52"/>
-      <c r="C63" s="37" t="s">
+      <c r="B63" s="74"/>
+      <c r="C63" s="60" t="s">
         <v>159</v>
       </c>
       <c r="D63" s="41" t="s">
@@ -5003,13 +5004,13 @@
       <c r="I63" s="23"/>
     </row>
     <row r="64" spans="1:9" s="30" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="34"/>
-      <c r="B64" s="52"/>
+      <c r="A64" s="47"/>
+      <c r="B64" s="74"/>
       <c r="C64" s="64"/>
-      <c r="D64" s="63" t="s">
+      <c r="D64" s="38" t="s">
         <v>157</v>
       </c>
-      <c r="E64" s="55"/>
+      <c r="E64" s="39"/>
       <c r="F64" s="25"/>
       <c r="G64" s="25" t="s">
         <v>158</v>
@@ -5022,11 +5023,11 @@
       </c>
     </row>
     <row r="65" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="34" t="s">
+      <c r="A65" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="B65" s="52"/>
-      <c r="C65" s="37" t="s">
+      <c r="B65" s="74"/>
+      <c r="C65" s="60" t="s">
         <v>160</v>
       </c>
       <c r="D65" s="41" t="s">
@@ -5039,13 +5040,13 @@
       <c r="I65" s="23"/>
     </row>
     <row r="66" spans="1:9" s="30" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="34"/>
-      <c r="B66" s="52"/>
-      <c r="C66" s="65"/>
-      <c r="D66" s="63" t="s">
+      <c r="A66" s="47"/>
+      <c r="B66" s="74"/>
+      <c r="C66" s="63"/>
+      <c r="D66" s="38" t="s">
         <v>157</v>
       </c>
-      <c r="E66" s="55"/>
+      <c r="E66" s="39"/>
       <c r="F66" s="32"/>
       <c r="G66" s="25" t="s">
         <v>158</v>
@@ -5058,11 +5059,11 @@
       </c>
     </row>
     <row r="67" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="34" t="s">
+      <c r="A67" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="B67" s="52"/>
-      <c r="C67" s="36" t="s">
+      <c r="B67" s="74"/>
+      <c r="C67" s="59" t="s">
         <v>161</v>
       </c>
       <c r="D67" s="41" t="s">
@@ -5075,13 +5076,13 @@
       <c r="I67" s="21"/>
     </row>
     <row r="68" spans="1:9" s="30" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="34"/>
-      <c r="B68" s="52"/>
-      <c r="C68" s="65"/>
-      <c r="D68" s="63" t="s">
+      <c r="A68" s="47"/>
+      <c r="B68" s="74"/>
+      <c r="C68" s="63"/>
+      <c r="D68" s="38" t="s">
         <v>157</v>
       </c>
-      <c r="E68" s="55"/>
+      <c r="E68" s="39"/>
       <c r="F68" s="32"/>
       <c r="G68" s="25" t="s">
         <v>158</v>
@@ -5094,11 +5095,11 @@
       </c>
     </row>
     <row r="69" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="34" t="s">
+      <c r="A69" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="B69" s="52"/>
-      <c r="C69" s="36" t="s">
+      <c r="B69" s="74"/>
+      <c r="C69" s="59" t="s">
         <v>162</v>
       </c>
       <c r="D69" s="41" t="s">
@@ -5111,13 +5112,13 @@
       <c r="I69" s="21"/>
     </row>
     <row r="70" spans="1:9" s="30" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="34"/>
-      <c r="B70" s="52"/>
-      <c r="C70" s="37"/>
-      <c r="D70" s="63" t="s">
+      <c r="A70" s="47"/>
+      <c r="B70" s="74"/>
+      <c r="C70" s="60"/>
+      <c r="D70" s="38" t="s">
         <v>157</v>
       </c>
-      <c r="E70" s="55"/>
+      <c r="E70" s="39"/>
       <c r="F70" s="32"/>
       <c r="G70" s="25" t="s">
         <v>158</v>
@@ -5130,11 +5131,11 @@
       </c>
     </row>
     <row r="71" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="34" t="s">
+      <c r="A71" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="B71" s="52"/>
-      <c r="C71" s="37" t="s">
+      <c r="B71" s="74"/>
+      <c r="C71" s="60" t="s">
         <v>163</v>
       </c>
       <c r="D71" s="41" t="s">
@@ -5147,13 +5148,13 @@
       <c r="I71" s="23"/>
     </row>
     <row r="72" spans="1:9" s="30" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="34"/>
-      <c r="B72" s="52"/>
+      <c r="A72" s="47"/>
+      <c r="B72" s="74"/>
       <c r="C72" s="64"/>
-      <c r="D72" s="63" t="s">
+      <c r="D72" s="38" t="s">
         <v>157</v>
       </c>
-      <c r="E72" s="55"/>
+      <c r="E72" s="39"/>
       <c r="F72" s="25"/>
       <c r="G72" s="25" t="s">
         <v>158</v>
@@ -5166,11 +5167,11 @@
       </c>
     </row>
     <row r="73" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="34" t="s">
+      <c r="A73" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="B73" s="52"/>
-      <c r="C73" s="37" t="s">
+      <c r="B73" s="74"/>
+      <c r="C73" s="60" t="s">
         <v>164</v>
       </c>
       <c r="D73" s="41" t="s">
@@ -5183,13 +5184,13 @@
       <c r="I73" s="23"/>
     </row>
     <row r="74" spans="1:9" s="30" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="34"/>
-      <c r="B74" s="52"/>
-      <c r="C74" s="65"/>
-      <c r="D74" s="63" t="s">
+      <c r="A74" s="47"/>
+      <c r="B74" s="74"/>
+      <c r="C74" s="63"/>
+      <c r="D74" s="38" t="s">
         <v>157</v>
       </c>
-      <c r="E74" s="55"/>
+      <c r="E74" s="39"/>
       <c r="F74" s="32"/>
       <c r="G74" s="25" t="s">
         <v>158</v>
@@ -5202,11 +5203,11 @@
       </c>
     </row>
     <row r="75" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="35" t="s">
+      <c r="A75" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="B75" s="52"/>
-      <c r="C75" s="38" t="s">
+      <c r="B75" s="74"/>
+      <c r="C75" s="61" t="s">
         <v>165</v>
       </c>
       <c r="D75" s="41" t="s">
@@ -5219,13 +5220,13 @@
       <c r="I75" s="21"/>
     </row>
     <row r="76" spans="1:9" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="45"/>
-      <c r="B76" s="52"/>
-      <c r="C76" s="53"/>
-      <c r="D76" s="63" t="s">
+      <c r="A76" s="69"/>
+      <c r="B76" s="74"/>
+      <c r="C76" s="75"/>
+      <c r="D76" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="E76" s="55"/>
+      <c r="E76" s="39"/>
       <c r="F76" s="21"/>
       <c r="G76" s="25" t="s">
         <v>139</v>
@@ -5236,13 +5237,13 @@
       <c r="I76" s="21"/>
     </row>
     <row r="77" spans="1:9" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="45"/>
-      <c r="B77" s="52"/>
-      <c r="C77" s="53"/>
-      <c r="D77" s="54" t="s">
+      <c r="A77" s="69"/>
+      <c r="B77" s="74"/>
+      <c r="C77" s="75"/>
+      <c r="D77" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="E77" s="55"/>
+      <c r="E77" s="39"/>
       <c r="F77" s="25"/>
       <c r="G77" s="25" t="s">
         <v>217</v>
@@ -5255,13 +5256,13 @@
       </c>
     </row>
     <row r="78" spans="1:9" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="34" t="s">
+      <c r="A78" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="B78" s="39" t="s">
+      <c r="B78" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="C78" s="37" t="s">
+      <c r="C78" s="60" t="s">
         <v>166</v>
       </c>
       <c r="D78" s="41" t="s">
@@ -5274,26 +5275,26 @@
       <c r="I78" s="26"/>
     </row>
     <row r="79" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="34"/>
-      <c r="B79" s="39"/>
-      <c r="C79" s="37"/>
-      <c r="D79" s="43" t="s">
+      <c r="A79" s="47"/>
+      <c r="B79" s="62"/>
+      <c r="C79" s="60"/>
+      <c r="D79" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="E79" s="44"/>
+      <c r="E79" s="35"/>
       <c r="F79" s="21"/>
       <c r="G79" s="21"/>
       <c r="H79" s="21"/>
       <c r="I79" s="21"/>
     </row>
     <row r="80" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="34"/>
-      <c r="B80" s="39"/>
-      <c r="C80" s="37"/>
-      <c r="D80" s="43" t="s">
+      <c r="A80" s="47"/>
+      <c r="B80" s="62"/>
+      <c r="C80" s="60"/>
+      <c r="D80" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="E80" s="44"/>
+      <c r="E80" s="35"/>
       <c r="F80" s="21"/>
       <c r="G80" s="21" t="s">
         <v>139</v>
@@ -5304,13 +5305,13 @@
       <c r="I80" s="21"/>
     </row>
     <row r="81" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="34"/>
-      <c r="B81" s="39"/>
-      <c r="C81" s="38"/>
-      <c r="D81" s="43" t="s">
+      <c r="A81" s="47"/>
+      <c r="B81" s="62"/>
+      <c r="C81" s="61"/>
+      <c r="D81" s="34" t="s">
         <v>223</v>
       </c>
-      <c r="E81" s="44"/>
+      <c r="E81" s="35"/>
       <c r="F81" s="21"/>
       <c r="G81" s="21" t="s">
         <v>217</v>
@@ -5323,11 +5324,11 @@
       </c>
     </row>
     <row r="82" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="34" t="s">
+      <c r="A82" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="B82" s="39"/>
-      <c r="C82" s="37" t="s">
+      <c r="B82" s="62"/>
+      <c r="C82" s="60" t="s">
         <v>167</v>
       </c>
       <c r="D82" s="41" t="s">
@@ -5340,26 +5341,26 @@
       <c r="I82" s="23"/>
     </row>
     <row r="83" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="34"/>
-      <c r="B83" s="39"/>
-      <c r="C83" s="37"/>
-      <c r="D83" s="43" t="s">
+      <c r="A83" s="47"/>
+      <c r="B83" s="62"/>
+      <c r="C83" s="60"/>
+      <c r="D83" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="E83" s="44"/>
+      <c r="E83" s="35"/>
       <c r="F83" s="21"/>
       <c r="G83" s="21"/>
       <c r="H83" s="21"/>
       <c r="I83" s="21"/>
     </row>
     <row r="84" spans="1:9" s="30" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="34"/>
-      <c r="B84" s="39"/>
-      <c r="C84" s="38"/>
-      <c r="D84" s="63" t="s">
+      <c r="A84" s="47"/>
+      <c r="B84" s="62"/>
+      <c r="C84" s="61"/>
+      <c r="D84" s="38" t="s">
         <v>224</v>
       </c>
-      <c r="E84" s="55"/>
+      <c r="E84" s="39"/>
       <c r="F84" s="25"/>
       <c r="G84" s="25" t="s">
         <v>152</v>
@@ -5372,11 +5373,11 @@
       </c>
     </row>
     <row r="85" spans="1:9" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="34" t="s">
+      <c r="A85" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="B85" s="39"/>
-      <c r="C85" s="37" t="s">
+      <c r="B85" s="62"/>
+      <c r="C85" s="60" t="s">
         <v>168</v>
       </c>
       <c r="D85" s="41" t="s">
@@ -5389,26 +5390,26 @@
       <c r="I85" s="26"/>
     </row>
     <row r="86" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="34"/>
-      <c r="B86" s="39"/>
-      <c r="C86" s="37"/>
-      <c r="D86" s="43" t="s">
+      <c r="A86" s="47"/>
+      <c r="B86" s="62"/>
+      <c r="C86" s="60"/>
+      <c r="D86" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="E86" s="44"/>
+      <c r="E86" s="35"/>
       <c r="F86" s="21"/>
       <c r="G86" s="21"/>
       <c r="H86" s="21"/>
       <c r="I86" s="21"/>
     </row>
     <row r="87" spans="1:9" s="30" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="34"/>
-      <c r="B87" s="39"/>
-      <c r="C87" s="38"/>
-      <c r="D87" s="63" t="s">
+      <c r="A87" s="47"/>
+      <c r="B87" s="62"/>
+      <c r="C87" s="61"/>
+      <c r="D87" s="38" t="s">
         <v>224</v>
       </c>
-      <c r="E87" s="55"/>
+      <c r="E87" s="39"/>
       <c r="F87" s="25"/>
       <c r="G87" s="25" t="s">
         <v>152</v>
@@ -5421,11 +5422,11 @@
       </c>
     </row>
     <row r="88" spans="1:9" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="34" t="s">
+      <c r="A88" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="B88" s="39"/>
-      <c r="C88" s="37" t="s">
+      <c r="B88" s="62"/>
+      <c r="C88" s="60" t="s">
         <v>169</v>
       </c>
       <c r="D88" s="41" t="s">
@@ -5438,26 +5439,26 @@
       <c r="I88" s="26"/>
     </row>
     <row r="89" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="34"/>
-      <c r="B89" s="39"/>
-      <c r="C89" s="37"/>
-      <c r="D89" s="43" t="s">
+      <c r="A89" s="47"/>
+      <c r="B89" s="62"/>
+      <c r="C89" s="60"/>
+      <c r="D89" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="E89" s="44"/>
+      <c r="E89" s="35"/>
       <c r="F89" s="21"/>
       <c r="G89" s="21"/>
       <c r="H89" s="21"/>
       <c r="I89" s="21"/>
     </row>
     <row r="90" spans="1:9" s="30" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="34"/>
-      <c r="B90" s="39"/>
-      <c r="C90" s="38"/>
-      <c r="D90" s="63" t="s">
+      <c r="A90" s="47"/>
+      <c r="B90" s="62"/>
+      <c r="C90" s="61"/>
+      <c r="D90" s="38" t="s">
         <v>224</v>
       </c>
-      <c r="E90" s="55"/>
+      <c r="E90" s="39"/>
       <c r="F90" s="25"/>
       <c r="G90" s="25" t="s">
         <v>152</v>
@@ -5470,11 +5471,11 @@
       </c>
     </row>
     <row r="91" spans="1:9" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="34" t="s">
+      <c r="A91" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="B91" s="39"/>
-      <c r="C91" s="37" t="s">
+      <c r="B91" s="62"/>
+      <c r="C91" s="60" t="s">
         <v>170</v>
       </c>
       <c r="D91" s="41" t="s">
@@ -5487,26 +5488,26 @@
       <c r="I91" s="26"/>
     </row>
     <row r="92" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="34"/>
-      <c r="B92" s="39"/>
-      <c r="C92" s="37"/>
-      <c r="D92" s="43" t="s">
+      <c r="A92" s="47"/>
+      <c r="B92" s="62"/>
+      <c r="C92" s="60"/>
+      <c r="D92" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="E92" s="44"/>
+      <c r="E92" s="35"/>
       <c r="F92" s="21"/>
       <c r="G92" s="21"/>
       <c r="H92" s="21"/>
       <c r="I92" s="21"/>
     </row>
     <row r="93" spans="1:9" s="30" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="34"/>
-      <c r="B93" s="39"/>
-      <c r="C93" s="37"/>
-      <c r="D93" s="66" t="s">
+      <c r="A93" s="47"/>
+      <c r="B93" s="62"/>
+      <c r="C93" s="60"/>
+      <c r="D93" s="43" t="s">
         <v>224</v>
       </c>
-      <c r="E93" s="51"/>
+      <c r="E93" s="44"/>
       <c r="F93" s="32"/>
       <c r="G93" s="32" t="s">
         <v>152</v>
@@ -5519,43 +5520,43 @@
       </c>
     </row>
     <row r="94" spans="1:9" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="34" t="s">
+      <c r="A94" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="B94" s="39"/>
-      <c r="C94" s="36" t="s">
+      <c r="B94" s="62"/>
+      <c r="C94" s="59" t="s">
         <v>171</v>
       </c>
-      <c r="D94" s="43" t="s">
+      <c r="D94" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="E94" s="44"/>
+      <c r="E94" s="35"/>
       <c r="F94" s="25"/>
       <c r="G94" s="25"/>
       <c r="H94" s="25"/>
       <c r="I94" s="25"/>
     </row>
     <row r="95" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="34"/>
-      <c r="B95" s="39"/>
-      <c r="C95" s="37"/>
-      <c r="D95" s="43" t="s">
+      <c r="A95" s="47"/>
+      <c r="B95" s="62"/>
+      <c r="C95" s="60"/>
+      <c r="D95" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="E95" s="44"/>
+      <c r="E95" s="35"/>
       <c r="F95" s="21"/>
       <c r="G95" s="21"/>
       <c r="H95" s="21"/>
       <c r="I95" s="21"/>
     </row>
     <row r="96" spans="1:9" s="30" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="34"/>
-      <c r="B96" s="39"/>
-      <c r="C96" s="37"/>
-      <c r="D96" s="66" t="s">
+      <c r="A96" s="47"/>
+      <c r="B96" s="62"/>
+      <c r="C96" s="60"/>
+      <c r="D96" s="43" t="s">
         <v>224</v>
       </c>
-      <c r="E96" s="51"/>
+      <c r="E96" s="44"/>
       <c r="F96" s="32"/>
       <c r="G96" s="32" t="s">
         <v>152</v>
@@ -5568,43 +5569,43 @@
       </c>
     </row>
     <row r="97" spans="1:9" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="34" t="s">
+      <c r="A97" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="B97" s="39"/>
-      <c r="C97" s="36" t="s">
+      <c r="B97" s="62"/>
+      <c r="C97" s="59" t="s">
         <v>172</v>
       </c>
-      <c r="D97" s="43" t="s">
+      <c r="D97" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="E97" s="44"/>
+      <c r="E97" s="35"/>
       <c r="F97" s="25"/>
       <c r="G97" s="25"/>
       <c r="H97" s="25"/>
       <c r="I97" s="25"/>
     </row>
     <row r="98" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="34"/>
-      <c r="B98" s="39"/>
-      <c r="C98" s="37"/>
-      <c r="D98" s="43" t="s">
+      <c r="A98" s="47"/>
+      <c r="B98" s="62"/>
+      <c r="C98" s="60"/>
+      <c r="D98" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="E98" s="44"/>
+      <c r="E98" s="35"/>
       <c r="F98" s="21"/>
       <c r="G98" s="21"/>
       <c r="H98" s="21"/>
       <c r="I98" s="21"/>
     </row>
     <row r="99" spans="1:9" s="30" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="34"/>
-      <c r="B99" s="39"/>
-      <c r="C99" s="37"/>
-      <c r="D99" s="63" t="s">
+      <c r="A99" s="47"/>
+      <c r="B99" s="62"/>
+      <c r="C99" s="60"/>
+      <c r="D99" s="38" t="s">
         <v>224</v>
       </c>
-      <c r="E99" s="55"/>
+      <c r="E99" s="39"/>
       <c r="F99" s="25"/>
       <c r="G99" s="25" t="s">
         <v>152</v>
@@ -5617,14 +5618,14 @@
       </c>
     </row>
     <row r="100" spans="1:9" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="35" t="s">
+      <c r="A100" s="72" t="s">
         <v>105</v>
       </c>
-      <c r="B100" s="39"/>
-      <c r="C100" s="47" t="s">
+      <c r="B100" s="62"/>
+      <c r="C100" s="76" t="s">
         <v>173</v>
       </c>
-      <c r="D100" s="56" t="s">
+      <c r="D100" s="71" t="s">
         <v>202</v>
       </c>
       <c r="E100" s="42"/>
@@ -5634,26 +5635,26 @@
       <c r="I100" s="26"/>
     </row>
     <row r="101" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="45"/>
-      <c r="B101" s="39"/>
-      <c r="C101" s="48"/>
-      <c r="D101" s="79" t="s">
+      <c r="A101" s="69"/>
+      <c r="B101" s="62"/>
+      <c r="C101" s="77"/>
+      <c r="D101" s="40" t="s">
         <v>221</v>
       </c>
-      <c r="E101" s="44"/>
+      <c r="E101" s="35"/>
       <c r="F101" s="21"/>
       <c r="G101" s="21"/>
       <c r="H101" s="21"/>
       <c r="I101" s="21"/>
     </row>
     <row r="102" spans="1:9" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="45"/>
-      <c r="B102" s="39"/>
-      <c r="C102" s="48"/>
-      <c r="D102" s="54" t="s">
+      <c r="A102" s="69"/>
+      <c r="B102" s="62"/>
+      <c r="C102" s="77"/>
+      <c r="D102" s="46" t="s">
         <v>222</v>
       </c>
-      <c r="E102" s="55"/>
+      <c r="E102" s="39"/>
       <c r="F102" s="25"/>
       <c r="G102" s="25" t="s">
         <v>139</v>
@@ -5664,13 +5665,13 @@
       <c r="I102" s="25"/>
     </row>
     <row r="103" spans="1:9" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="46"/>
-      <c r="B103" s="39"/>
-      <c r="C103" s="49"/>
-      <c r="D103" s="50" t="s">
+      <c r="A103" s="70"/>
+      <c r="B103" s="62"/>
+      <c r="C103" s="78"/>
+      <c r="D103" s="79" t="s">
         <v>223</v>
       </c>
-      <c r="E103" s="51"/>
+      <c r="E103" s="44"/>
       <c r="F103" s="32"/>
       <c r="G103" s="32"/>
       <c r="H103" s="32"/>
@@ -5679,43 +5680,43 @@
       </c>
     </row>
     <row r="104" spans="1:9" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="34" t="s">
+      <c r="A104" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="B104" s="39"/>
-      <c r="C104" s="36" t="s">
+      <c r="B104" s="62"/>
+      <c r="C104" s="59" t="s">
         <v>176</v>
       </c>
-      <c r="D104" s="43" t="s">
+      <c r="D104" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="E104" s="44"/>
+      <c r="E104" s="35"/>
       <c r="F104" s="25"/>
       <c r="G104" s="25"/>
       <c r="H104" s="25"/>
       <c r="I104" s="25"/>
     </row>
     <row r="105" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="34"/>
-      <c r="B105" s="39"/>
-      <c r="C105" s="37"/>
-      <c r="D105" s="43" t="s">
+      <c r="A105" s="47"/>
+      <c r="B105" s="62"/>
+      <c r="C105" s="60"/>
+      <c r="D105" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="E105" s="44"/>
+      <c r="E105" s="35"/>
       <c r="F105" s="21"/>
       <c r="G105" s="21"/>
       <c r="H105" s="21"/>
       <c r="I105" s="21"/>
     </row>
     <row r="106" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="35"/>
-      <c r="B106" s="40"/>
-      <c r="C106" s="38"/>
-      <c r="D106" s="43" t="s">
+      <c r="A106" s="72"/>
+      <c r="B106" s="73"/>
+      <c r="C106" s="61"/>
+      <c r="D106" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="E106" s="44"/>
+      <c r="E106" s="35"/>
       <c r="F106" s="21"/>
       <c r="G106" s="21" t="s">
         <v>175</v>
@@ -5728,13 +5729,13 @@
       </c>
     </row>
     <row r="107" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="34" t="s">
+      <c r="A107" s="47" t="s">
         <v>107</v>
       </c>
-      <c r="B107" s="39" t="s">
+      <c r="B107" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="C107" s="37" t="s">
+      <c r="C107" s="60" t="s">
         <v>185</v>
       </c>
       <c r="D107" s="41" t="s">
@@ -5747,26 +5748,26 @@
       <c r="I107" s="23"/>
     </row>
     <row r="108" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="34"/>
-      <c r="B108" s="39"/>
-      <c r="C108" s="37"/>
-      <c r="D108" s="43" t="s">
+      <c r="A108" s="47"/>
+      <c r="B108" s="62"/>
+      <c r="C108" s="60"/>
+      <c r="D108" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="E108" s="44"/>
+      <c r="E108" s="35"/>
       <c r="F108" s="21"/>
       <c r="G108" s="21"/>
       <c r="H108" s="21"/>
       <c r="I108" s="21"/>
     </row>
     <row r="109" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="34"/>
-      <c r="B109" s="39"/>
-      <c r="C109" s="37"/>
-      <c r="D109" s="43" t="s">
+      <c r="A109" s="47"/>
+      <c r="B109" s="62"/>
+      <c r="C109" s="60"/>
+      <c r="D109" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="E109" s="44"/>
+      <c r="E109" s="35"/>
       <c r="F109" s="21"/>
       <c r="G109" s="21" t="s">
         <v>139</v>
@@ -5777,13 +5778,13 @@
       <c r="I109" s="21"/>
     </row>
     <row r="110" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="34"/>
-      <c r="B110" s="39"/>
-      <c r="C110" s="38"/>
-      <c r="D110" s="43" t="s">
+      <c r="A110" s="47"/>
+      <c r="B110" s="62"/>
+      <c r="C110" s="61"/>
+      <c r="D110" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="E110" s="44"/>
+      <c r="E110" s="35"/>
       <c r="F110" s="21"/>
       <c r="G110" s="21" t="s">
         <v>177</v>
@@ -5796,11 +5797,11 @@
       </c>
     </row>
     <row r="111" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="34" t="s">
+      <c r="A111" s="47" t="s">
         <v>116</v>
       </c>
-      <c r="B111" s="39"/>
-      <c r="C111" s="37" t="s">
+      <c r="B111" s="62"/>
+      <c r="C111" s="60" t="s">
         <v>186</v>
       </c>
       <c r="D111" s="41" t="s">
@@ -5813,26 +5814,26 @@
       <c r="I111" s="23"/>
     </row>
     <row r="112" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="34"/>
-      <c r="B112" s="39"/>
-      <c r="C112" s="37"/>
-      <c r="D112" s="43" t="s">
+      <c r="A112" s="47"/>
+      <c r="B112" s="62"/>
+      <c r="C112" s="60"/>
+      <c r="D112" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="E112" s="44"/>
+      <c r="E112" s="35"/>
       <c r="F112" s="21"/>
       <c r="G112" s="21"/>
       <c r="H112" s="21"/>
       <c r="I112" s="21"/>
     </row>
     <row r="113" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="34"/>
-      <c r="B113" s="39"/>
-      <c r="C113" s="37"/>
-      <c r="D113" s="43" t="s">
+      <c r="A113" s="47"/>
+      <c r="B113" s="62"/>
+      <c r="C113" s="60"/>
+      <c r="D113" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="E113" s="44"/>
+      <c r="E113" s="35"/>
       <c r="F113" s="21"/>
       <c r="G113" s="21" t="s">
         <v>139</v>
@@ -5843,13 +5844,13 @@
       <c r="I113" s="21"/>
     </row>
     <row r="114" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="34"/>
-      <c r="B114" s="39"/>
-      <c r="C114" s="38"/>
-      <c r="D114" s="43" t="s">
+      <c r="A114" s="47"/>
+      <c r="B114" s="62"/>
+      <c r="C114" s="61"/>
+      <c r="D114" s="34" t="s">
         <v>228</v>
       </c>
-      <c r="E114" s="44"/>
+      <c r="E114" s="35"/>
       <c r="F114" s="21"/>
       <c r="G114" s="21" t="s">
         <v>178</v>
@@ -5862,11 +5863,11 @@
       </c>
     </row>
     <row r="115" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="34" t="s">
+      <c r="A115" s="47" t="s">
         <v>117</v>
       </c>
-      <c r="B115" s="39"/>
-      <c r="C115" s="37" t="s">
+      <c r="B115" s="62"/>
+      <c r="C115" s="60" t="s">
         <v>187</v>
       </c>
       <c r="D115" s="41" t="s">
@@ -5879,26 +5880,26 @@
       <c r="I115" s="23"/>
     </row>
     <row r="116" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="34"/>
-      <c r="B116" s="39"/>
-      <c r="C116" s="37"/>
-      <c r="D116" s="43" t="s">
+      <c r="A116" s="47"/>
+      <c r="B116" s="62"/>
+      <c r="C116" s="60"/>
+      <c r="D116" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="E116" s="44"/>
+      <c r="E116" s="35"/>
       <c r="F116" s="21"/>
       <c r="G116" s="21"/>
       <c r="H116" s="21"/>
       <c r="I116" s="21"/>
     </row>
     <row r="117" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="34"/>
-      <c r="B117" s="39"/>
-      <c r="C117" s="37"/>
-      <c r="D117" s="43" t="s">
+      <c r="A117" s="47"/>
+      <c r="B117" s="62"/>
+      <c r="C117" s="60"/>
+      <c r="D117" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="E117" s="44"/>
+      <c r="E117" s="35"/>
       <c r="F117" s="21"/>
       <c r="G117" s="21" t="s">
         <v>139</v>
@@ -5909,13 +5910,13 @@
       <c r="I117" s="21"/>
     </row>
     <row r="118" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="34"/>
-      <c r="B118" s="39"/>
-      <c r="C118" s="38"/>
-      <c r="D118" s="43" t="s">
+      <c r="A118" s="47"/>
+      <c r="B118" s="62"/>
+      <c r="C118" s="61"/>
+      <c r="D118" s="34" t="s">
         <v>229</v>
       </c>
-      <c r="E118" s="44"/>
+      <c r="E118" s="35"/>
       <c r="F118" s="21"/>
       <c r="G118" s="21" t="s">
         <v>179</v>
@@ -5928,11 +5929,11 @@
       </c>
     </row>
     <row r="119" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="34" t="s">
+      <c r="A119" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="B119" s="39"/>
-      <c r="C119" s="37" t="s">
+      <c r="B119" s="62"/>
+      <c r="C119" s="60" t="s">
         <v>188</v>
       </c>
       <c r="D119" s="41" t="s">
@@ -5945,26 +5946,26 @@
       <c r="I119" s="23"/>
     </row>
     <row r="120" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="34"/>
-      <c r="B120" s="39"/>
-      <c r="C120" s="37"/>
-      <c r="D120" s="43" t="s">
+      <c r="A120" s="47"/>
+      <c r="B120" s="62"/>
+      <c r="C120" s="60"/>
+      <c r="D120" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="E120" s="44"/>
+      <c r="E120" s="35"/>
       <c r="F120" s="21"/>
       <c r="G120" s="21"/>
       <c r="H120" s="21"/>
       <c r="I120" s="21"/>
     </row>
     <row r="121" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="34"/>
-      <c r="B121" s="39"/>
-      <c r="C121" s="37"/>
-      <c r="D121" s="43" t="s">
+      <c r="A121" s="47"/>
+      <c r="B121" s="62"/>
+      <c r="C121" s="60"/>
+      <c r="D121" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="E121" s="44"/>
+      <c r="E121" s="35"/>
       <c r="F121" s="21"/>
       <c r="G121" s="21" t="s">
         <v>139</v>
@@ -5975,13 +5976,13 @@
       <c r="I121" s="21"/>
     </row>
     <row r="122" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="34"/>
-      <c r="B122" s="39"/>
-      <c r="C122" s="38"/>
-      <c r="D122" s="43" t="s">
+      <c r="A122" s="47"/>
+      <c r="B122" s="62"/>
+      <c r="C122" s="61"/>
+      <c r="D122" s="34" t="s">
         <v>230</v>
       </c>
-      <c r="E122" s="44"/>
+      <c r="E122" s="35"/>
       <c r="F122" s="21"/>
       <c r="G122" s="21" t="s">
         <v>180</v>
@@ -5994,11 +5995,11 @@
       </c>
     </row>
     <row r="123" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="34" t="s">
+      <c r="A123" s="47" t="s">
         <v>119</v>
       </c>
-      <c r="B123" s="39"/>
-      <c r="C123" s="37" t="s">
+      <c r="B123" s="62"/>
+      <c r="C123" s="60" t="s">
         <v>189</v>
       </c>
       <c r="D123" s="41" t="s">
@@ -6011,26 +6012,26 @@
       <c r="I123" s="23"/>
     </row>
     <row r="124" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="34"/>
-      <c r="B124" s="39"/>
-      <c r="C124" s="37"/>
-      <c r="D124" s="43" t="s">
+      <c r="A124" s="47"/>
+      <c r="B124" s="62"/>
+      <c r="C124" s="60"/>
+      <c r="D124" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="E124" s="44"/>
+      <c r="E124" s="35"/>
       <c r="F124" s="21"/>
       <c r="G124" s="21"/>
       <c r="H124" s="21"/>
       <c r="I124" s="21"/>
     </row>
     <row r="125" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="34"/>
-      <c r="B125" s="39"/>
-      <c r="C125" s="37"/>
-      <c r="D125" s="43" t="s">
+      <c r="A125" s="47"/>
+      <c r="B125" s="62"/>
+      <c r="C125" s="60"/>
+      <c r="D125" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="E125" s="44"/>
+      <c r="E125" s="35"/>
       <c r="F125" s="21"/>
       <c r="G125" s="21" t="s">
         <v>139</v>
@@ -6041,13 +6042,13 @@
       <c r="I125" s="21"/>
     </row>
     <row r="126" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="34"/>
-      <c r="B126" s="39"/>
-      <c r="C126" s="37"/>
-      <c r="D126" s="57" t="s">
+      <c r="A126" s="47"/>
+      <c r="B126" s="62"/>
+      <c r="C126" s="60"/>
+      <c r="D126" s="36" t="s">
         <v>231</v>
       </c>
-      <c r="E126" s="58"/>
+      <c r="E126" s="37"/>
       <c r="F126" s="24"/>
       <c r="G126" s="24" t="s">
         <v>181</v>
@@ -6060,43 +6061,43 @@
       </c>
     </row>
     <row r="127" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="34" t="s">
+      <c r="A127" s="47" t="s">
         <v>120</v>
       </c>
-      <c r="B127" s="39"/>
-      <c r="C127" s="36" t="s">
+      <c r="B127" s="62"/>
+      <c r="C127" s="59" t="s">
         <v>190</v>
       </c>
-      <c r="D127" s="43" t="s">
+      <c r="D127" s="34" t="s">
         <v>208</v>
       </c>
-      <c r="E127" s="44"/>
+      <c r="E127" s="35"/>
       <c r="F127" s="21"/>
       <c r="G127" s="21"/>
       <c r="H127" s="21"/>
       <c r="I127" s="21"/>
     </row>
     <row r="128" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="34"/>
-      <c r="B128" s="39"/>
-      <c r="C128" s="37"/>
-      <c r="D128" s="43" t="s">
+      <c r="A128" s="47"/>
+      <c r="B128" s="62"/>
+      <c r="C128" s="60"/>
+      <c r="D128" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="E128" s="44"/>
+      <c r="E128" s="35"/>
       <c r="F128" s="21"/>
       <c r="G128" s="21"/>
       <c r="H128" s="21"/>
       <c r="I128" s="21"/>
     </row>
     <row r="129" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="34"/>
-      <c r="B129" s="39"/>
-      <c r="C129" s="37"/>
-      <c r="D129" s="43" t="s">
+      <c r="A129" s="47"/>
+      <c r="B129" s="62"/>
+      <c r="C129" s="60"/>
+      <c r="D129" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="E129" s="44"/>
+      <c r="E129" s="35"/>
       <c r="F129" s="21"/>
       <c r="G129" s="21" t="s">
         <v>139</v>
@@ -6107,13 +6108,13 @@
       <c r="I129" s="21"/>
     </row>
     <row r="130" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="34"/>
-      <c r="B130" s="39"/>
-      <c r="C130" s="37"/>
-      <c r="D130" s="57" t="s">
+      <c r="A130" s="47"/>
+      <c r="B130" s="62"/>
+      <c r="C130" s="60"/>
+      <c r="D130" s="36" t="s">
         <v>232</v>
       </c>
-      <c r="E130" s="58"/>
+      <c r="E130" s="37"/>
       <c r="F130" s="24"/>
       <c r="G130" s="24" t="s">
         <v>182</v>
@@ -6126,43 +6127,43 @@
       </c>
     </row>
     <row r="131" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="34" t="s">
+      <c r="A131" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="B131" s="39"/>
-      <c r="C131" s="36" t="s">
+      <c r="B131" s="62"/>
+      <c r="C131" s="59" t="s">
         <v>191</v>
       </c>
-      <c r="D131" s="43" t="s">
+      <c r="D131" s="34" t="s">
         <v>209</v>
       </c>
-      <c r="E131" s="44"/>
+      <c r="E131" s="35"/>
       <c r="F131" s="21"/>
       <c r="G131" s="21"/>
       <c r="H131" s="21"/>
       <c r="I131" s="21"/>
     </row>
     <row r="132" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="34"/>
-      <c r="B132" s="39"/>
-      <c r="C132" s="37"/>
-      <c r="D132" s="43" t="s">
+      <c r="A132" s="47"/>
+      <c r="B132" s="62"/>
+      <c r="C132" s="60"/>
+      <c r="D132" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="E132" s="44"/>
+      <c r="E132" s="35"/>
       <c r="F132" s="21"/>
       <c r="G132" s="21"/>
       <c r="H132" s="21"/>
       <c r="I132" s="21"/>
     </row>
     <row r="133" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="34"/>
-      <c r="B133" s="39"/>
-      <c r="C133" s="37"/>
-      <c r="D133" s="43" t="s">
+      <c r="A133" s="47"/>
+      <c r="B133" s="62"/>
+      <c r="C133" s="60"/>
+      <c r="D133" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="E133" s="44"/>
+      <c r="E133" s="35"/>
       <c r="F133" s="21"/>
       <c r="G133" s="21" t="s">
         <v>139</v>
@@ -6173,13 +6174,13 @@
       <c r="I133" s="21"/>
     </row>
     <row r="134" spans="1:9" s="30" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="34"/>
-      <c r="B134" s="39"/>
-      <c r="C134" s="37"/>
-      <c r="D134" s="66" t="s">
+      <c r="A134" s="47"/>
+      <c r="B134" s="62"/>
+      <c r="C134" s="60"/>
+      <c r="D134" s="43" t="s">
         <v>233</v>
       </c>
-      <c r="E134" s="51"/>
+      <c r="E134" s="44"/>
       <c r="F134" s="32"/>
       <c r="G134" s="32" t="s">
         <v>183</v>
@@ -6192,43 +6193,43 @@
       </c>
     </row>
     <row r="135" spans="1:9" s="30" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="34" t="s">
+      <c r="A135" s="47" t="s">
         <v>122</v>
       </c>
-      <c r="B135" s="39"/>
-      <c r="C135" s="36" t="s">
+      <c r="B135" s="62"/>
+      <c r="C135" s="59" t="s">
         <v>192</v>
       </c>
-      <c r="D135" s="43" t="s">
+      <c r="D135" s="34" t="s">
         <v>210</v>
       </c>
-      <c r="E135" s="44"/>
+      <c r="E135" s="35"/>
       <c r="F135" s="25"/>
       <c r="G135" s="25"/>
       <c r="H135" s="25"/>
       <c r="I135" s="25"/>
     </row>
     <row r="136" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="34"/>
-      <c r="B136" s="39"/>
-      <c r="C136" s="37"/>
-      <c r="D136" s="43" t="s">
+      <c r="A136" s="47"/>
+      <c r="B136" s="62"/>
+      <c r="C136" s="60"/>
+      <c r="D136" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="E136" s="44"/>
+      <c r="E136" s="35"/>
       <c r="F136" s="21"/>
       <c r="G136" s="21"/>
       <c r="H136" s="21"/>
       <c r="I136" s="21"/>
     </row>
     <row r="137" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="34"/>
-      <c r="B137" s="39"/>
-      <c r="C137" s="37"/>
-      <c r="D137" s="57" t="s">
+      <c r="A137" s="47"/>
+      <c r="B137" s="62"/>
+      <c r="C137" s="60"/>
+      <c r="D137" s="36" t="s">
         <v>222</v>
       </c>
-      <c r="E137" s="58"/>
+      <c r="E137" s="37"/>
       <c r="F137" s="24"/>
       <c r="G137" s="24" t="s">
         <v>139</v>
@@ -6241,39 +6242,39 @@
       </c>
     </row>
     <row r="138" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="34" t="s">
+      <c r="A138" s="47" t="s">
         <v>124</v>
       </c>
-      <c r="B138" s="39"/>
-      <c r="C138" s="36" t="s">
+      <c r="B138" s="62"/>
+      <c r="C138" s="59" t="s">
         <v>193</v>
       </c>
-      <c r="D138" s="43" t="s">
+      <c r="D138" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="E138" s="44"/>
+      <c r="E138" s="35"/>
       <c r="F138" s="21"/>
       <c r="G138" s="21"/>
       <c r="H138" s="21"/>
       <c r="I138" s="21"/>
     </row>
     <row r="139" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="34"/>
-      <c r="B139" s="39"/>
-      <c r="C139" s="37"/>
-      <c r="D139" s="43" t="s">
+      <c r="A139" s="47"/>
+      <c r="B139" s="62"/>
+      <c r="C139" s="60"/>
+      <c r="D139" s="34" t="s">
         <v>226</v>
       </c>
-      <c r="E139" s="44"/>
+      <c r="E139" s="35"/>
       <c r="F139" s="21"/>
       <c r="G139" s="21"/>
       <c r="H139" s="21"/>
       <c r="I139" s="21"/>
     </row>
     <row r="140" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A140" s="34"/>
-      <c r="B140" s="39"/>
-      <c r="C140" s="37"/>
+      <c r="A140" s="47"/>
+      <c r="B140" s="62"/>
+      <c r="C140" s="60"/>
       <c r="D140" s="31" t="s">
         <v>174</v>
       </c>
@@ -6290,13 +6291,13 @@
       </c>
     </row>
     <row r="141" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="34" t="s">
+      <c r="A141" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="B141" s="39" t="s">
+      <c r="B141" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="C141" s="37" t="s">
+      <c r="C141" s="60" t="s">
         <v>219</v>
       </c>
       <c r="D141" s="41" t="s">
@@ -6309,26 +6310,26 @@
       <c r="I141" s="23"/>
     </row>
     <row r="142" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="34"/>
-      <c r="B142" s="39"/>
-      <c r="C142" s="37"/>
-      <c r="D142" s="43" t="s">
+      <c r="A142" s="47"/>
+      <c r="B142" s="62"/>
+      <c r="C142" s="60"/>
+      <c r="D142" s="34" t="s">
         <v>234</v>
       </c>
-      <c r="E142" s="44"/>
+      <c r="E142" s="35"/>
       <c r="F142" s="21"/>
       <c r="G142" s="21"/>
       <c r="H142" s="21"/>
       <c r="I142" s="21"/>
     </row>
     <row r="143" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="34"/>
-      <c r="B143" s="39"/>
-      <c r="C143" s="38"/>
-      <c r="D143" s="43" t="s">
+      <c r="A143" s="47"/>
+      <c r="B143" s="62"/>
+      <c r="C143" s="61"/>
+      <c r="D143" s="34" t="s">
         <v>235</v>
       </c>
-      <c r="E143" s="44"/>
+      <c r="E143" s="35"/>
       <c r="F143" s="21"/>
       <c r="G143" s="21" t="s">
         <v>195</v>
@@ -6341,11 +6342,11 @@
       </c>
     </row>
     <row r="144" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="34" t="s">
+      <c r="A144" s="47" t="s">
         <v>218</v>
       </c>
-      <c r="B144" s="39"/>
-      <c r="C144" s="37" t="s">
+      <c r="B144" s="62"/>
+      <c r="C144" s="60" t="s">
         <v>220</v>
       </c>
       <c r="D144" s="41" t="s">
@@ -6358,26 +6359,26 @@
       <c r="I144" s="23"/>
     </row>
     <row r="145" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="34"/>
-      <c r="B145" s="39"/>
-      <c r="C145" s="37"/>
-      <c r="D145" s="43" t="s">
+      <c r="A145" s="47"/>
+      <c r="B145" s="62"/>
+      <c r="C145" s="60"/>
+      <c r="D145" s="34" t="s">
         <v>234</v>
       </c>
-      <c r="E145" s="44"/>
+      <c r="E145" s="35"/>
       <c r="F145" s="21"/>
       <c r="G145" s="21"/>
       <c r="H145" s="21"/>
       <c r="I145" s="21"/>
     </row>
     <row r="146" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A146" s="34"/>
-      <c r="B146" s="39"/>
-      <c r="C146" s="37"/>
-      <c r="D146" s="57" t="s">
+      <c r="A146" s="47"/>
+      <c r="B146" s="62"/>
+      <c r="C146" s="60"/>
+      <c r="D146" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="E146" s="58"/>
+      <c r="E146" s="37"/>
       <c r="F146" s="24"/>
       <c r="G146" s="24" t="s">
         <v>175</v>
@@ -6390,32 +6391,32 @@
       </c>
     </row>
     <row r="147" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A147" s="45" t="s">
+      <c r="A147" s="69" t="s">
         <v>196</v>
       </c>
-      <c r="B147" s="61" t="s">
+      <c r="B147" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="C147" s="59" t="s">
+      <c r="C147" s="65" t="s">
         <v>197</v>
       </c>
-      <c r="D147" s="79" t="s">
+      <c r="D147" s="40" t="s">
         <v>198</v>
       </c>
-      <c r="E147" s="44"/>
+      <c r="E147" s="35"/>
       <c r="F147" s="21"/>
       <c r="G147" s="21"/>
       <c r="H147" s="21"/>
       <c r="I147" s="21"/>
     </row>
     <row r="148" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A148" s="46"/>
-      <c r="B148" s="62"/>
-      <c r="C148" s="60"/>
-      <c r="D148" s="78" t="s">
+      <c r="A148" s="70"/>
+      <c r="B148" s="68"/>
+      <c r="C148" s="66"/>
+      <c r="D148" s="45" t="s">
         <v>194</v>
       </c>
-      <c r="E148" s="58"/>
+      <c r="E148" s="37"/>
       <c r="F148" s="24"/>
       <c r="G148" s="24" t="s">
         <v>195</v>
@@ -7201,182 +7202,34 @@
     <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="251">
-    <mergeCell ref="D113:E113"/>
-    <mergeCell ref="D146:E146"/>
-    <mergeCell ref="D145:E145"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="D101:E101"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="D133:E133"/>
-    <mergeCell ref="D144:E144"/>
-    <mergeCell ref="D138:E138"/>
-    <mergeCell ref="D141:E141"/>
-    <mergeCell ref="D131:E131"/>
-    <mergeCell ref="D135:E135"/>
-    <mergeCell ref="D122:E122"/>
-    <mergeCell ref="D129:E129"/>
-    <mergeCell ref="D130:E130"/>
-    <mergeCell ref="D132:E132"/>
-    <mergeCell ref="D134:E134"/>
-    <mergeCell ref="D136:E136"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="D119:E119"/>
-    <mergeCell ref="D148:E148"/>
-    <mergeCell ref="D147:E147"/>
-    <mergeCell ref="D121:E121"/>
-    <mergeCell ref="D124:E124"/>
-    <mergeCell ref="D125:E125"/>
-    <mergeCell ref="D126:E126"/>
-    <mergeCell ref="D128:E128"/>
-    <mergeCell ref="D116:E116"/>
-    <mergeCell ref="D117:E117"/>
-    <mergeCell ref="D118:E118"/>
-    <mergeCell ref="D120:E120"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="D102:E102"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="A85:A87"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B9:B23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="C60:C62"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="C48:C50"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D142:E142"/>
-    <mergeCell ref="D143:E143"/>
-    <mergeCell ref="C147:C148"/>
-    <mergeCell ref="B147:B148"/>
-    <mergeCell ref="A147:A148"/>
-    <mergeCell ref="A131:A134"/>
-    <mergeCell ref="C131:C134"/>
-    <mergeCell ref="C135:C137"/>
-    <mergeCell ref="A135:A137"/>
-    <mergeCell ref="A138:A140"/>
-    <mergeCell ref="C138:C140"/>
-    <mergeCell ref="C141:C143"/>
-    <mergeCell ref="C144:C146"/>
-    <mergeCell ref="B141:B146"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="A144:A146"/>
-    <mergeCell ref="D137:E137"/>
-    <mergeCell ref="D139:E139"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="D104:E104"/>
+    <mergeCell ref="A127:A130"/>
+    <mergeCell ref="C127:C130"/>
+    <mergeCell ref="B107:B140"/>
+    <mergeCell ref="A100:A103"/>
+    <mergeCell ref="C100:C103"/>
+    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="C85:C87"/>
+    <mergeCell ref="C88:C90"/>
+    <mergeCell ref="C107:C110"/>
+    <mergeCell ref="A107:A110"/>
+    <mergeCell ref="C111:C114"/>
+    <mergeCell ref="C115:C118"/>
+    <mergeCell ref="C119:C122"/>
+    <mergeCell ref="C123:C126"/>
+    <mergeCell ref="A111:A114"/>
+    <mergeCell ref="A115:A118"/>
+    <mergeCell ref="A119:A122"/>
+    <mergeCell ref="A123:A126"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="B60:B77"/>
+    <mergeCell ref="C75:C77"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="C73:C74"/>
     <mergeCell ref="C82:C84"/>
     <mergeCell ref="A82:A84"/>
     <mergeCell ref="A51:A53"/>
@@ -7401,11 +7254,152 @@
     <mergeCell ref="D77:E77"/>
     <mergeCell ref="A78:A81"/>
     <mergeCell ref="C78:C81"/>
+    <mergeCell ref="C147:C148"/>
+    <mergeCell ref="B147:B148"/>
+    <mergeCell ref="A147:A148"/>
+    <mergeCell ref="A131:A134"/>
+    <mergeCell ref="C131:C134"/>
+    <mergeCell ref="C135:C137"/>
+    <mergeCell ref="A135:A137"/>
+    <mergeCell ref="A138:A140"/>
+    <mergeCell ref="C138:C140"/>
+    <mergeCell ref="C141:C143"/>
+    <mergeCell ref="C144:C146"/>
+    <mergeCell ref="B141:B146"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A144:A146"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="C60:C62"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="C57:C59"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B9:B23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="B24:B59"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D74:E74"/>
     <mergeCell ref="D79:E79"/>
     <mergeCell ref="D82:E82"/>
     <mergeCell ref="D85:E85"/>
     <mergeCell ref="D88:E88"/>
     <mergeCell ref="D91:E91"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="D102:E102"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="A85:A87"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="D104:E104"/>
     <mergeCell ref="D94:E94"/>
     <mergeCell ref="D93:E93"/>
     <mergeCell ref="A88:A90"/>
@@ -7415,43 +7409,50 @@
     <mergeCell ref="A94:A96"/>
     <mergeCell ref="A97:A99"/>
     <mergeCell ref="C97:C99"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="C57:C59"/>
-    <mergeCell ref="B24:B59"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="B60:B77"/>
-    <mergeCell ref="C75:C77"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="C73:C74"/>
     <mergeCell ref="A104:A106"/>
     <mergeCell ref="C104:C106"/>
     <mergeCell ref="B78:B106"/>
-    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="D148:E148"/>
+    <mergeCell ref="D147:E147"/>
+    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="D124:E124"/>
+    <mergeCell ref="D125:E125"/>
+    <mergeCell ref="D126:E126"/>
+    <mergeCell ref="D128:E128"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="D117:E117"/>
+    <mergeCell ref="D118:E118"/>
+    <mergeCell ref="D120:E120"/>
+    <mergeCell ref="D142:E142"/>
+    <mergeCell ref="D143:E143"/>
+    <mergeCell ref="D137:E137"/>
+    <mergeCell ref="D139:E139"/>
     <mergeCell ref="D123:E123"/>
     <mergeCell ref="D127:E127"/>
-    <mergeCell ref="C107:C110"/>
-    <mergeCell ref="A107:A110"/>
-    <mergeCell ref="C111:C114"/>
-    <mergeCell ref="C115:C118"/>
-    <mergeCell ref="C119:C122"/>
-    <mergeCell ref="C123:C126"/>
-    <mergeCell ref="A111:A114"/>
-    <mergeCell ref="A115:A118"/>
-    <mergeCell ref="A119:A122"/>
-    <mergeCell ref="A123:A126"/>
-    <mergeCell ref="A127:A130"/>
-    <mergeCell ref="C127:C130"/>
-    <mergeCell ref="B107:B140"/>
-    <mergeCell ref="A100:A103"/>
-    <mergeCell ref="C100:C103"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="C85:C87"/>
-    <mergeCell ref="C88:C90"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="D146:E146"/>
+    <mergeCell ref="D145:E145"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="D101:E101"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="D133:E133"/>
+    <mergeCell ref="D144:E144"/>
+    <mergeCell ref="D138:E138"/>
+    <mergeCell ref="D141:E141"/>
+    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="D135:E135"/>
+    <mergeCell ref="D122:E122"/>
+    <mergeCell ref="D129:E129"/>
+    <mergeCell ref="D130:E130"/>
+    <mergeCell ref="D132:E132"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="D136:E136"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="D119:E119"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="D107:E107"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>